<commit_message>
added Indiana humanities info
</commit_message>
<xml_diff>
--- a/BTAA Positions.xlsx
+++ b/BTAA Positions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rutgersconnect-my.sharepoint.com/personal/rwomack_libraries_rutgers_edu/Documents/NBL/Exploratory/BTAAreview/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="189" documentId="11_9AE2215215EAAB2E32578452246B36726781E623" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C24A430B-740C-FA40-B8B2-929AB1136F8F}"/>
+  <xr:revisionPtr revIDLastSave="223" documentId="11_9AE2215215EAAB2E32578452246B36726781E623" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B6BDF33-A4EA-414F-8F6D-3CF7015F5BFF}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="500" windowWidth="26960" windowHeight="14440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="362">
   <si>
     <t>Social Sciences</t>
   </si>
@@ -678,9 +678,6 @@
     <t>Information Literacy &amp; Assessment Librarian</t>
   </si>
   <si>
-    <t>Director, Lilly Library</t>
-  </si>
-  <si>
     <t>Social Science &amp; Public Policy</t>
   </si>
   <si>
@@ -1069,6 +1066,51 @@
   </si>
   <si>
     <t>Asian</t>
+  </si>
+  <si>
+    <t>Humanities</t>
+  </si>
+  <si>
+    <t>SCUA</t>
+  </si>
+  <si>
+    <t>Sciences</t>
+  </si>
+  <si>
+    <t>Head of Sciences</t>
+  </si>
+  <si>
+    <t>Science Librarian</t>
+  </si>
+  <si>
+    <t>Head, Lilly Library</t>
+  </si>
+  <si>
+    <t>Art, Architecture, and Design Librarian</t>
+  </si>
+  <si>
+    <t>Librarian for English &amp; American Literature, Comparative Literature, and Theatre &amp; Drama</t>
+  </si>
+  <si>
+    <t>History Librarian</t>
+  </si>
+  <si>
+    <t>Librarian for Germanic Studies, French &amp; Italian, History &amp; Philosophy of Science, Classical Studies, and Linguistics</t>
+  </si>
+  <si>
+    <t>Director, Music Library</t>
+  </si>
+  <si>
+    <t>Associate Director and Head of Music Library Technical Services</t>
+  </si>
+  <si>
+    <t>Electronic Music Resources Librarian</t>
+  </si>
+  <si>
+    <t>Head, Education Library</t>
+  </si>
+  <si>
+    <t>Research &amp; Instruction Librarian, Business/SPEA</t>
   </si>
 </sst>
 </file>
@@ -1455,10 +1497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O91"/>
+  <dimension ref="A1:O101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G46" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L50" sqref="L50"/>
+    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -1537,8 +1579,8 @@
       <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E3" t="s">
-        <v>242</v>
+      <c r="E3" s="2" t="s">
+        <v>241</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>8</v>
@@ -1547,16 +1589,16 @@
         <v>93</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>68</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>68</v>
@@ -1573,11 +1615,14 @@
       <c r="B4" s="2" t="s">
         <v>168</v>
       </c>
+      <c r="C4" s="2" t="s">
+        <v>361</v>
+      </c>
       <c r="D4" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>68</v>
@@ -1586,10 +1631,10 @@
         <v>68</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>68</v>
@@ -1631,7 +1676,7 @@
         <v>68</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="N6" s="2" t="s">
         <v>58</v>
@@ -1643,7 +1688,7 @@
         <v>68</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="8" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1652,7 +1697,7 @@
         <v>68</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="9" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1678,10 +1723,10 @@
         <v>184</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>109</v>
@@ -1690,13 +1735,13 @@
         <v>94</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="L11" s="6" t="s">
         <v>116</v>
@@ -1710,14 +1755,17 @@
     </row>
     <row r="12" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="6" t="s">
         <v>167</v>
       </c>
+      <c r="C12" s="6" t="s">
+        <v>360</v>
+      </c>
       <c r="D12" s="6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>110</v>
@@ -1726,10 +1774,10 @@
         <v>96</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="K12" s="6" t="s">
         <v>100</v>
@@ -1747,10 +1795,10 @@
         <v>169</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>111</v>
@@ -1759,16 +1807,16 @@
         <v>97</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="O13" s="6" t="s">
         <v>14</v>
@@ -1779,14 +1827,14 @@
       <c r="B14" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="6" t="s">
         <v>185</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>112</v>
@@ -1795,13 +1843,13 @@
         <v>98</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="L14" s="6" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="O14" s="6" t="s">
         <v>15</v>
@@ -1813,7 +1861,7 @@
         <v>171</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>114</v>
@@ -1822,16 +1870,16 @@
         <v>99</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="16" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="E16" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>115</v>
@@ -1840,25 +1888,25 @@
         <v>100</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="L16" s="6" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="17" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="E17" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>116</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="L17" s="6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="18" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -1867,10 +1915,10 @@
         <v>117</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="L18" s="6" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
@@ -1889,10 +1937,10 @@
         <v>199</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>118</v>
@@ -1901,16 +1949,16 @@
         <v>103</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="M20" s="2" t="s">
         <v>69</v>
@@ -1928,13 +1976,13 @@
         <v>175</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>200</v>
+        <v>132</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>118</v>
@@ -1943,16 +1991,16 @@
         <v>105</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="M21" s="2" t="s">
         <v>74</v>
@@ -1970,10 +2018,10 @@
         <v>178</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>132</v>
+        <v>201</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>106</v>
@@ -1985,16 +2033,16 @@
         <v>107</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="N22" s="2" t="s">
         <v>52</v>
@@ -2009,10 +2057,10 @@
         <v>179</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>120</v>
@@ -2021,16 +2069,16 @@
         <v>106</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="N23" s="2" t="s">
         <v>54</v>
@@ -2045,7 +2093,7 @@
         <v>180</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>211</v>
@@ -2057,16 +2105,16 @@
         <v>106</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="O24" s="2" t="s">
         <v>21</v>
@@ -2078,22 +2126,22 @@
         <v>181</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>125</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="O25" s="2" t="s">
         <v>27</v>
@@ -2105,22 +2153,22 @@
         <v>181</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>126</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="O26" s="2" t="s">
         <v>34</v>
@@ -2129,19 +2177,19 @@
     <row r="27" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="C27" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>127</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="O27" s="2" t="s">
         <v>23</v>
@@ -2150,7 +2198,7 @@
     <row r="28" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="C28" s="2" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>210</v>
@@ -2159,10 +2207,10 @@
         <v>128</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="O28" s="2" t="s">
         <v>25</v>
@@ -2170,14 +2218,11 @@
     </row>
     <row r="29" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
-      <c r="C29" s="2" t="s">
-        <v>216</v>
-      </c>
       <c r="F29" s="2" t="s">
         <v>132</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="O29" s="2" t="s">
         <v>25</v>
@@ -2189,7 +2234,7 @@
         <v>136</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="O30" s="2" t="s">
         <v>26</v>
@@ -2211,11 +2256,11 @@
       <c r="C32" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>223</v>
+      <c r="D32" s="6" t="s">
+        <v>222</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F32" s="6" t="s">
         <v>139</v>
@@ -2224,16 +2269,16 @@
         <v>95</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="I32" s="6" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="K32" s="6" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="L32" s="6" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="M32" s="6" t="s">
         <v>66</v>
@@ -2251,13 +2296,13 @@
         <v>174</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>217</v>
+        <v>196</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F33" s="6" t="s">
         <v>123</v>
@@ -2266,10 +2311,10 @@
         <v>46</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I33" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="K33" s="6" t="s">
         <v>49</v>
@@ -2293,13 +2338,13 @@
         <v>49</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F34" s="6" t="s">
         <v>124</v>
@@ -2308,16 +2353,16 @@
         <v>101</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I34" s="6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="K34" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="L34" s="6" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="M34" s="6" t="s">
         <v>73</v>
@@ -2335,10 +2380,10 @@
         <v>176</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F35" s="6" t="s">
         <v>141</v>
@@ -2347,16 +2392,16 @@
         <v>102</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="I35" s="6" t="s">
         <v>207</v>
       </c>
       <c r="K35" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L35" s="6" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="N35" s="6" t="s">
         <v>49</v>
@@ -2371,10 +2416,10 @@
         <v>138</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F36" s="6" t="s">
         <v>129</v>
@@ -2383,13 +2428,13 @@
         <v>104</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K36" s="6" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="L36" s="6" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="N36" s="6" t="s">
         <v>53</v>
@@ -2404,7 +2449,7 @@
         <v>177</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="D37" s="6" t="s">
         <v>102</v>
@@ -2416,10 +2461,10 @@
         <v>108</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="L37" s="6" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="O37" s="6" t="s">
         <v>32</v>
@@ -2431,7 +2476,7 @@
         <v>182</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D38" s="6" t="s">
         <v>102</v>
@@ -2440,10 +2485,10 @@
         <v>131</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="L38" s="6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="O38" s="6" t="s">
         <v>33</v>
@@ -2452,7 +2497,7 @@
     <row r="39" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
       <c r="C39" s="6" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>207</v>
@@ -2461,73 +2506,73 @@
         <v>133</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="L39" s="6" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="40" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="C40" s="6" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F40" s="6" t="s">
         <v>134</v>
       </c>
       <c r="L40" s="6" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="41" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="C41" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F41" s="6" t="s">
         <v>135</v>
       </c>
       <c r="L41" s="6" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="42" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="C42" s="6" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="F42" s="6" t="s">
         <v>122</v>
       </c>
       <c r="L42" s="6" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="43" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="7"/>
       <c r="C43" s="6" t="s">
-        <v>213</v>
+        <v>195</v>
       </c>
       <c r="F43" s="6" t="s">
         <v>138</v>
       </c>
       <c r="L43" s="6" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="44" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="7"/>
       <c r="C44" s="6" t="s">
-        <v>195</v>
+        <v>214</v>
       </c>
     </row>
     <row r="45" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
       <c r="C45" s="6" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F45" s="6" t="s">
         <v>142</v>
@@ -2535,9 +2580,6 @@
     </row>
     <row r="46" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7"/>
-      <c r="C46" s="6" t="s">
-        <v>215</v>
-      </c>
       <c r="F46" s="6" t="s">
         <v>140</v>
       </c>
@@ -2553,7 +2595,7 @@
         <v>192</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F47" s="9" t="s">
         <v>148</v>
@@ -2562,10 +2604,10 @@
         <v>83</v>
       </c>
       <c r="H47" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K47" s="9" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="O47" s="9" t="s">
         <v>38</v>
@@ -2577,7 +2619,7 @@
         <v>84</v>
       </c>
       <c r="K48" s="9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="49" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -2592,13 +2634,13 @@
         <v>86</v>
       </c>
       <c r="H49" s="9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="K49" s="9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="L49" s="9" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="N49" s="9" t="s">
         <v>37</v>
@@ -2657,10 +2699,10 @@
         <v>88</v>
       </c>
       <c r="H53" s="9" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K53" s="9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="O53" s="9" t="s">
         <v>40</v>
@@ -2693,7 +2735,7 @@
         <v>90</v>
       </c>
       <c r="H56" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="57" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -2704,7 +2746,7 @@
         <v>92</v>
       </c>
       <c r="K57" s="9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="O57" s="9" t="s">
         <v>42</v>
@@ -2743,13 +2785,13 @@
         <v>91</v>
       </c>
       <c r="H61" s="9" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="K61" s="9" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L61" s="9" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="O61" s="9" t="s">
         <v>44</v>
@@ -2763,16 +2805,16 @@
         <v>187</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F62" s="9" t="s">
         <v>154</v>
       </c>
       <c r="H62" s="9" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I62" s="9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="63" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -2784,7 +2826,7 @@
       </c>
     </row>
     <row r="64" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="65" spans="2:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B65" s="9" t="s">
         <v>162</v>
       </c>
@@ -2798,21 +2840,21 @@
         <v>85</v>
       </c>
       <c r="H65" s="9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="K65" s="9" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="66" spans="2:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F66" s="9" t="s">
         <v>150</v>
       </c>
       <c r="H66" s="9" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="67" spans="2:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B67" s="9" t="s">
         <v>156</v>
       </c>
@@ -2823,49 +2865,136 @@
         <v>143</v>
       </c>
       <c r="I67" s="9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="K67" s="9" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="6" t="s">
+        <v>347</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C69" s="6" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C70" s="6" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C71" s="6" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C72" s="6" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C73" s="6" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C74" s="6" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C75" s="6" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="77" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="78" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="9" t="s">
+        <v>348</v>
+      </c>
+      <c r="C78" s="9" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C79" s="9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="81" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="82" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="83" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="84" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="85" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="86" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="87" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C88" s="2" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C89" s="2" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="91" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="92" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="93" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B86" t="s">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B87" t="s">
+    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B97" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B88" t="s">
+    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B98" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B89" t="s">
+    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B99" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B90" t="s">
+    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B100" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B91" t="s">
+    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B101" t="s">
         <v>70</v>
       </c>
     </row>

</xml_diff>

<commit_message>
small corrections git push qq() quit oedke
</commit_message>
<xml_diff>
--- a/BTAA Positions.xlsx
+++ b/BTAA Positions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rutgersconnect-my.sharepoint.com/personal/rwomack_libraries_rutgers_edu/Documents/NBL/Exploratory/BTAAreview/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="223" documentId="11_9AE2215215EAAB2E32578452246B36726781E623" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B6BDF33-A4EA-414F-8F6D-3CF7015F5BFF}"/>
+  <xr:revisionPtr revIDLastSave="228" documentId="11_9AE2215215EAAB2E32578452246B36726781E623" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6EB9F11-06E0-F247-A838-8670920587E7}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="363">
   <si>
     <t>Social Sciences</t>
   </si>
@@ -1111,6 +1111,9 @@
   </si>
   <si>
     <t>Research &amp; Instruction Librarian, Business/SPEA</t>
+  </si>
+  <si>
+    <t>Science Data Specialist (w/Chemistry &amp; Physics)</t>
   </si>
 </sst>
 </file>
@@ -1499,8 +1502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" topLeftCell="J32" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N38" sqref="N38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -2080,9 +2083,6 @@
       <c r="L23" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="N23" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="O23" s="2" t="s">
         <v>24</v>
       </c>
@@ -2466,6 +2466,9 @@
       <c r="L37" s="6" t="s">
         <v>331</v>
       </c>
+      <c r="N37" s="6" t="s">
+        <v>54</v>
+      </c>
       <c r="O37" s="6" t="s">
         <v>32</v>
       </c>
@@ -2489,6 +2492,9 @@
       </c>
       <c r="L38" s="6" t="s">
         <v>332</v>
+      </c>
+      <c r="N38" s="6" t="s">
+        <v>362</v>
       </c>
       <c r="O38" s="6" t="s">
         <v>33</v>

</xml_diff>